<commit_message>
coding style, meeting minutes
</commit_message>
<xml_diff>
--- a/Meeting_minutes/Coding_style.xlsx
+++ b/Meeting_minutes/Coding_style.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VLAD\IT\DAN_IT\FEM3-FINAL-PROJECT\Meeting_minutes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2264FE6F-920A-4458-AEA8-21E5B35C9DD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9EF34-596B-45A5-91AA-E4FEAC5B4232}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{16D8559A-848E-45EF-923F-FA620C3FB4E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,15 +34,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Event is called "event"</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>No JSX files (use js)</t>
+    <t>Event is called "event" (not "e", not "evt")</t>
+  </si>
+  <si>
+    <t>No JSX files - use only js</t>
+  </si>
+  <si>
+    <t>Arrow function inside functions. Main function (which is exported) - function declaration</t>
+  </si>
+  <si>
+    <t>Code should be self-explainable, comments can be used only to help in navigation</t>
+  </si>
+  <si>
+    <t>Language of team written communication - English</t>
+  </si>
+  <si>
+    <t>Site language - English</t>
+  </si>
+  <si>
+    <t>Database - MongoDB</t>
+  </si>
+  <si>
+    <t>Tab === 2 spaces</t>
+  </si>
+  <si>
+    <t>Classes naming: 3-4 words max, using "-" as word separator or camelCase in css in JS. Should describe element</t>
+  </si>
+  <si>
+    <t>Breakpoints: 768px and 1200px</t>
+  </si>
+  <si>
+    <t>Sprint - 1 week.</t>
+  </si>
+  <si>
+    <t>Weekly meeting with Mentor</t>
+  </si>
+  <si>
+    <t>At least 1 weekly offline meeting</t>
+  </si>
+  <si>
+    <t>Using PropTypes and Default Props</t>
+  </si>
+  <si>
+    <t>Ajax requests are written in "services" folder</t>
+  </si>
+  <si>
+    <t>Forbidden to push to branch "develop" code with eslint errors</t>
+  </si>
+  <si>
+    <t>Forbidden to push to branch "develop" code with red errors/warnings in concole</t>
+  </si>
+  <si>
+    <t>Mobile first approach in site layout</t>
+  </si>
+  <si>
+    <t>Branch develop and master are protected</t>
+  </si>
+  <si>
+    <t>Daily calls at 10:30 (except weekends)</t>
+  </si>
+  <si>
+    <t>Icons we take preferably from Material UI</t>
+  </si>
+  <si>
+    <t>Each component should have separate folder. If component has subcomponents, which can’t be used anywhere else – we create folder in folder</t>
+  </si>
+  <si>
+    <t>Only css in js (withStyle, makeStyle, styled components)</t>
+  </si>
+  <si>
+    <t>Files with styles are called with “_” at the beginning.</t>
+  </si>
+  <si>
+    <t>React Hooks (do not use classes)</t>
+  </si>
+  <si>
+    <t>Punctuation</t>
+  </si>
+  <si>
+    <t>Files/Folders</t>
+  </si>
+  <si>
+    <t>JS code</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>Styling</t>
+  </si>
+  <si>
+    <t>MUI</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Adaptive</t>
+  </si>
+  <si>
+    <t>Files' names start with small letter using "-" as word separator.</t>
+  </si>
+  <si>
+    <t>Components folders are named with capital letter and using "-" as word separator.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Maximum is done using Material UI (where it's possible)</t>
+  </si>
+  <si>
+    <t>Maybe later we can try Flow?</t>
+  </si>
+  <si>
+    <t>We use Redux</t>
+  </si>
+  <si>
+    <t>SCRUM</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -58,22 +178,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,20 +207,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,36 +566,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A25FB06-5BD7-4B86-AC89-EF62D95CEC3C}">
-  <dimension ref="B1:B3"/>
+  <dimension ref="B1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="35.21875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="47.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:4" s="1" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>2</v>
-      </c>
+    <row r="17" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:C1" xr:uid="{A7BDE6F0-7801-4CBF-92DA-5E26543D0FD9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C30">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>